<commit_message>
more than 1 branch added, admin page updated accordingly
</commit_message>
<xml_diff>
--- a/Other Files/EEE_2021-2025.xlsx
+++ b/Other Files/EEE_2021-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noelm\Documents\PROJECTS\A10dance\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9B9122-F9FF-45ED-B338-BCC9EA6A47A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE51E70-A20B-4080-A979-2758AB2F1551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>U2105048</t>
   </si>
   <si>
-    <t xml:space="preserve">u2105036 </t>
+    <t xml:space="preserve">U2105036 </t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>